<commit_message>
Remove Logo; Changed Titles; Required Input
</commit_message>
<xml_diff>
--- a/findComps/Comp Tables/Competitive Market.xlsx
+++ b/findComps/Comp Tables/Competitive Market.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
   <si>
     <t>Facility Name</t>
   </si>
@@ -70,55 +70,220 @@
     <t>S</t>
   </si>
   <si>
-    <t>Seven Hills Health &amp; Rehab Center</t>
-  </si>
-  <si>
-    <t>819 ROCKSIDE ROAD</t>
-  </si>
-  <si>
-    <t>Seven Hills</t>
+    <t>Metrohealth System</t>
+  </si>
+  <si>
+    <t>2500 METROHEALTH DRIVE</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
   </si>
   <si>
     <t>OH</t>
   </si>
   <si>
-    <t>44131</t>
-  </si>
-  <si>
-    <t>2166745482</t>
+    <t>44109</t>
+  </si>
+  <si>
+    <t>2167783792</t>
   </si>
   <si>
     <t>SNF</t>
   </si>
   <si>
-    <t>12.0 mi</t>
+    <t>7.0 mi</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Joshua Tree Care Center</t>
+  </si>
+  <si>
+    <t>27500 MILL RD</t>
+  </si>
+  <si>
+    <t>North Olmsted</t>
+  </si>
+  <si>
+    <t>44070</t>
+  </si>
+  <si>
+    <t>4407778444</t>
+  </si>
+  <si>
+    <t>9.9 mi</t>
+  </si>
+  <si>
+    <t>Enniscourt Nursing Care</t>
+  </si>
+  <si>
+    <t>13315 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>Lakewood</t>
+  </si>
+  <si>
+    <t>44107</t>
+  </si>
+  <si>
+    <t>2162263858</t>
+  </si>
+  <si>
+    <t>2.5 mi</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Franklin Plaza Extended Care</t>
+  </si>
+  <si>
+    <t>3600 FRANKLIN BOULEVARD</t>
+  </si>
+  <si>
+    <t>44113</t>
+  </si>
+  <si>
+    <t>2166511600</t>
+  </si>
+  <si>
+    <t>6.3 mi</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Joshua Tree Care Center</t>
-  </si>
-  <si>
-    <t>27500 MILL RD</t>
-  </si>
-  <si>
-    <t>North Olmsted</t>
-  </si>
-  <si>
-    <t>44070</t>
-  </si>
-  <si>
-    <t>4407778444</t>
-  </si>
-  <si>
-    <t>12.4 mi</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>Rae-Ann West Park</t>
+  </si>
+  <si>
+    <t>4650 ROCKY RIVER DR</t>
+  </si>
+  <si>
+    <t>44135</t>
+  </si>
+  <si>
+    <t>2162675445</t>
+  </si>
+  <si>
+    <t>3.0 mi</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Berea Center</t>
+  </si>
+  <si>
+    <t>49 SHELDON RD</t>
+  </si>
+  <si>
+    <t>Berea</t>
+  </si>
+  <si>
+    <t>44017</t>
+  </si>
+  <si>
+    <t>4402340454</t>
+  </si>
+  <si>
+    <t>6.9 mi</t>
+  </si>
+  <si>
+    <t>Century Oak Care Center</t>
+  </si>
+  <si>
+    <t>7250 OLD OAK BLVD</t>
+  </si>
+  <si>
+    <t>Middleburg Heights</t>
+  </si>
+  <si>
+    <t>44130</t>
+  </si>
+  <si>
+    <t>4402437888</t>
+  </si>
+  <si>
+    <t>8.4 mi</t>
+  </si>
+  <si>
+    <t>Normandy Manor Of Rocky River</t>
+  </si>
+  <si>
+    <t>22709 LAKE RD</t>
+  </si>
+  <si>
+    <t>Rocky River</t>
+  </si>
+  <si>
+    <t>44116</t>
+  </si>
+  <si>
+    <t>4403335400</t>
+  </si>
+  <si>
+    <t>5.1 mi</t>
+  </si>
+  <si>
+    <t>Pleasant Lake Villa</t>
+  </si>
+  <si>
+    <t>7260 RIDGE RD</t>
+  </si>
+  <si>
+    <t>Parma</t>
+  </si>
+  <si>
+    <t>44129</t>
+  </si>
+  <si>
+    <t>4408422273</t>
+  </si>
+  <si>
+    <t>12.6 mi</t>
+  </si>
+  <si>
+    <t>Health Center At The Renaissan</t>
+  </si>
+  <si>
+    <t>26376 JOHN RD</t>
+  </si>
+  <si>
+    <t>Olmsted Twp</t>
+  </si>
+  <si>
+    <t>44138</t>
+  </si>
+  <si>
+    <t>4402357100</t>
+  </si>
+  <si>
+    <t>10.9 mi</t>
+  </si>
+  <si>
+    <t>O'Neill Healthcare Fairview Park</t>
+  </si>
+  <si>
+    <t>20770 LORAIN ROAD</t>
+  </si>
+  <si>
+    <t>Fairview Park</t>
+  </si>
+  <si>
+    <t>44126</t>
+  </si>
+  <si>
+    <t>4403310300</t>
+  </si>
+  <si>
+    <t>3.3 mi</t>
   </si>
   <si>
     <t>Mt Alverna Home Inc</t>
@@ -127,79 +292,19 @@
     <t>6765 STATE ROAD</t>
   </si>
   <si>
-    <t>Parma</t>
-  </si>
-  <si>
     <t>44134</t>
   </si>
   <si>
     <t>4408437800</t>
   </si>
   <si>
-    <t>14.1 mi</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Villa Camillus  The</t>
-  </si>
-  <si>
-    <t>10515 E RIVER RD</t>
-  </si>
-  <si>
-    <t>Columbia Station</t>
-  </si>
-  <si>
-    <t>44028</t>
-  </si>
-  <si>
-    <t>4402365091</t>
-  </si>
-  <si>
-    <t>14.7 mi</t>
-  </si>
-  <si>
-    <t>Pleasantview Care Center</t>
-  </si>
-  <si>
-    <t>7377 RIDGE RD</t>
-  </si>
-  <si>
-    <t>44129</t>
-  </si>
-  <si>
-    <t>4408450200</t>
-  </si>
-  <si>
-    <t>10.5 mi</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Larchwood Village Retirement Community</t>
-  </si>
-  <si>
-    <t>4110 ROCKY RIVER DRIVE</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
-    <t>44135</t>
-  </si>
-  <si>
-    <t>2169416100</t>
-  </si>
-  <si>
-    <t>4.4 mi</t>
-  </si>
-  <si>
-    <t>North Park Care Center</t>
-  </si>
-  <si>
-    <t>14801 HOLLAND ROAD</t>
+    <t>14.3 mi</t>
+  </si>
+  <si>
+    <t>East Park Care Center</t>
+  </si>
+  <si>
+    <t>8 EAST PARK CIRCLE</t>
   </si>
   <si>
     <t>Brook Park</t>
@@ -208,253 +313,25 @@
     <t>44142</t>
   </si>
   <si>
-    <t>2168031995</t>
-  </si>
-  <si>
-    <t>10.1 mi</t>
-  </si>
-  <si>
-    <t>Franklin Plaza Extended Care</t>
-  </si>
-  <si>
-    <t>3600 FRANKLIN BOULEVARD</t>
-  </si>
-  <si>
-    <t>44113</t>
-  </si>
-  <si>
-    <t>2166511600</t>
-  </si>
-  <si>
-    <t>4.5 mi</t>
-  </si>
-  <si>
-    <t>Riverview Pointe Care Center</t>
-  </si>
-  <si>
-    <t>9027 COLUMBIA ROAD</t>
-  </si>
-  <si>
-    <t>Olmsted Falls</t>
-  </si>
-  <si>
-    <t>44138</t>
-  </si>
-  <si>
-    <t>4404278884</t>
-  </si>
-  <si>
-    <t>Welsh Home The</t>
-  </si>
-  <si>
-    <t>22199 CENTER RIDGE RD</t>
-  </si>
-  <si>
-    <t>Rocky River</t>
-  </si>
-  <si>
-    <t>44116</t>
-  </si>
-  <si>
-    <t>4403310420</t>
-  </si>
-  <si>
-    <t>5.9 mi</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Lakewood</t>
-  </si>
-  <si>
-    <t>13900 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>Lakewood</t>
-  </si>
-  <si>
-    <t>44107</t>
-  </si>
-  <si>
-    <t>2162287650</t>
-  </si>
-  <si>
-    <t>0.3 mi</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Diplomat Healthcare</t>
-  </si>
-  <si>
-    <t>9001 W 130TH ST</t>
-  </si>
-  <si>
-    <t>North Royalton</t>
-  </si>
-  <si>
-    <t>44133</t>
-  </si>
-  <si>
-    <t>4402373104</t>
-  </si>
-  <si>
-    <t>14.5 mi</t>
-  </si>
-  <si>
-    <t>Falling Water Healthcare Center</t>
-  </si>
-  <si>
-    <t>18840 FALLING WATER</t>
-  </si>
-  <si>
-    <t>Strongsville</t>
-  </si>
-  <si>
-    <t>44136</t>
-  </si>
-  <si>
-    <t>4402381100</t>
-  </si>
-  <si>
-    <t>14.3 mi</t>
-  </si>
-  <si>
-    <t>Elisabeth Sev Prentiss Ctr For</t>
-  </si>
-  <si>
-    <t>3525 SCRANTON ROAD</t>
-  </si>
-  <si>
-    <t>44109</t>
-  </si>
-  <si>
-    <t>2169578090</t>
-  </si>
-  <si>
-    <t>8.0 mi</t>
-  </si>
-  <si>
-    <t>Aristocrat Berea Nursing Home</t>
-  </si>
-  <si>
-    <t>255 FRONT STREET</t>
-  </si>
-  <si>
-    <t>Berea</t>
-  </si>
-  <si>
-    <t>44017</t>
-  </si>
-  <si>
-    <t>4402434000</t>
-  </si>
-  <si>
-    <t>11.1 mi</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Fairview Park</t>
-  </si>
-  <si>
-    <t>20770 LORAIN ROAD</t>
-  </si>
-  <si>
-    <t>Fairview Park</t>
-  </si>
-  <si>
-    <t>44126</t>
-  </si>
-  <si>
-    <t>4403310300</t>
-  </si>
-  <si>
-    <t>5.4 mi</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Bay Village</t>
-  </si>
-  <si>
-    <t>605 BRADLEY RD</t>
-  </si>
-  <si>
-    <t>Bay Village</t>
-  </si>
-  <si>
-    <t>44140</t>
-  </si>
-  <si>
-    <t>4408713474</t>
-  </si>
-  <si>
-    <t>11.2 mi</t>
-  </si>
-  <si>
-    <t>Algart Health Care</t>
-  </si>
-  <si>
-    <t>8902 DETROIT AVE</t>
+    <t>2162677229</t>
+  </si>
+  <si>
+    <t>7.7 mi</t>
+  </si>
+  <si>
+    <t>St Augustine Manor</t>
+  </si>
+  <si>
+    <t>7801 DETROIT AVE</t>
   </si>
   <si>
     <t>44102</t>
   </si>
   <si>
-    <t>2166311550</t>
-  </si>
-  <si>
-    <t>1.9 mi</t>
-  </si>
-  <si>
-    <t>West Bay Care And Rehab Center</t>
-  </si>
-  <si>
-    <t>27601 WESTCHESTER PKWY</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>44145</t>
-  </si>
-  <si>
-    <t>4408715900</t>
-  </si>
-  <si>
-    <t>10.2 mi</t>
-  </si>
-  <si>
-    <t>Heights Care And Rehab Center, The</t>
-  </si>
-  <si>
-    <t>2801 E ROYALTON RD</t>
-  </si>
-  <si>
-    <t>Broadview Heights</t>
-  </si>
-  <si>
-    <t>44147</t>
-  </si>
-  <si>
-    <t>4405264770</t>
-  </si>
-  <si>
-    <t>20.3 mi</t>
-  </si>
-  <si>
-    <t>Southern Hills Health And Reha</t>
-  </si>
-  <si>
-    <t>19530 BAGLEY ROAD</t>
-  </si>
-  <si>
-    <t>Middleburg Heights</t>
-  </si>
-  <si>
-    <t>44130</t>
-  </si>
-  <si>
-    <t>4408167500</t>
-  </si>
-  <si>
-    <t>11.5 mi</t>
+    <t>2166347400</t>
+  </si>
+  <si>
+    <t>4.7 mi</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +958,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>24</v>
@@ -1090,13 +967,13 @@
         <v>0</v>
       </c>
       <c r="L2" s="24" t="n">
-        <v>0.0625</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="M2" s="24" t="b">
         <v>0</v>
       </c>
       <c r="N2" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="24" t="b">
         <v>0</v>
@@ -1159,7 +1036,7 @@
         <v>25</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1168,49 +1045,49 @@
         <v/>
       </c>
       <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="J4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M4" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="24" t="s">
         <v>39</v>
-      </c>
-      <c r="K4" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="24" t="n">
-        <v>0.9607843137254902</v>
-      </c>
-      <c r="M4" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>40</v>
@@ -1228,46 +1105,46 @@
         <v>42</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="J5" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="26" t="n">
+        <v>0.7910447761194029</v>
+      </c>
+      <c r="M5" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="19" t="s">
         <v>46</v>
-      </c>
-      <c r="K5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="26" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="M5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1282,7 +1159,7 @@
         <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
@@ -1297,7 +1174,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="8" t="n">
-        <v>162</v>
+        <v>70</v>
       </c>
       <c r="J6" s="27" t="s">
         <v>51</v>
@@ -1306,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="24" t="n">
-        <v>0.8765432098765432</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="M6" s="24" t="b">
         <v>0</v>
@@ -1318,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1351,7 +1228,7 @@
         <v>23</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>58</v>
@@ -1360,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="26" t="n">
-        <v>0.7676767676767676</v>
+        <v>0.9</v>
       </c>
       <c r="M7" s="26" t="b">
         <v>0</v>
@@ -1372,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1405,7 +1282,7 @@
         <v>23</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="J8" s="27" t="s">
         <v>64</v>
@@ -1414,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="24" t="n">
-        <v>0.92</v>
+        <v>0.6391752577319587</v>
       </c>
       <c r="M8" s="24" t="b">
         <v>0</v>
@@ -1429,7 +1306,7 @@
         <v>25</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1444,31 +1321,31 @@
         <v>66</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K9" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="26" t="n">
-        <v>0.7910447761194029</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="M9" s="26" t="b">
         <v>0</v>
@@ -1480,10 +1357,10 @@
         <v>0</v>
       </c>
       <c r="P9" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1492,37 +1369,37 @@
         <v/>
       </c>
       <c r="B10" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="8" t="n">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="K10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L10" s="24" t="n">
-        <v>0.9603960396039604</v>
+        <v>0.914572864321608</v>
       </c>
       <c r="M10" s="24" t="b">
         <v>0</v>
@@ -1534,10 +1411,10 @@
         <v>0</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1546,40 +1423,40 @@
         <v/>
       </c>
       <c r="B11" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="15" t="n">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K11" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L11" s="26" t="n">
-        <v>0.9113924050632911</v>
+        <v>0.9270833333333334</v>
       </c>
       <c r="M11" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="26" t="b">
         <v>0</v>
@@ -1588,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="P11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="Q11" s="19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1600,40 +1477,40 @@
         <v/>
       </c>
       <c r="B12" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="8" t="n">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K12" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L12" s="24" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="M12" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="24" t="b">
         <v>0</v>
@@ -1642,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>26</v>
@@ -1654,13 +1531,13 @@
         <v/>
       </c>
       <c r="B13" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>20</v>
@@ -1675,7 +1552,7 @@
         <v>23</v>
       </c>
       <c r="I13" s="15" t="n">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>93</v>
@@ -1684,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="26" t="n">
-        <v>0.9461538461538461</v>
+        <v>0.9607843137254902</v>
       </c>
       <c r="M13" s="26" t="b">
         <v>0</v>
@@ -1699,7 +1576,7 @@
         <v>25</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1729,7 +1606,7 @@
         <v>23</v>
       </c>
       <c r="I14" s="8" t="n">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>99</v>
@@ -1738,10 +1615,10 @@
         <v>0</v>
       </c>
       <c r="L14" s="24" t="n">
-        <v>0.8518518518518519</v>
+        <v>0.6825396825396826</v>
       </c>
       <c r="M14" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="24" t="b">
         <v>0</v>
@@ -1750,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1768,7 +1645,7 @@
         <v>101</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>20</v>
@@ -1783,7 +1660,7 @@
         <v>23</v>
       </c>
       <c r="I15" s="15" t="n">
-        <v>150</v>
+        <v>248</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>104</v>
@@ -1792,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="26" t="n">
-        <v>0.9533333333333334</v>
+        <v>0.875</v>
       </c>
       <c r="M15" s="26" t="b">
         <v>0</v>
@@ -1815,378 +1692,154 @@
         <f>A15+1</f>
         <v/>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="8" t="n">
-        <v>165</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K16" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="24" t="n">
-        <v>0.9515151515151515</v>
-      </c>
-      <c r="M16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P16" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
+      <c r="D16" s="6" t="n"/>
+      <c r="E16" s="6" t="n"/>
+      <c r="F16" s="9" t="n"/>
+      <c r="G16" s="9" t="n"/>
+      <c r="H16" s="9" t="n"/>
+      <c r="I16" s="8" t="n"/>
+      <c r="J16" s="9" t="n"/>
+      <c r="K16" s="10" t="n"/>
+      <c r="L16" s="24" t="n"/>
+      <c r="M16" s="24" t="n"/>
+      <c r="N16" s="24" t="n"/>
+      <c r="O16" s="24" t="n"/>
+      <c r="P16" s="24" t="n"/>
+      <c r="Q16" s="12" t="n"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="5">
         <f>A16+1</f>
         <v/>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="15" t="n">
-        <v>118</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M17" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O17" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P17" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q17" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="B17" s="13" t="n"/>
+      <c r="C17" s="13" t="n"/>
+      <c r="D17" s="13" t="n"/>
+      <c r="E17" s="13" t="n"/>
+      <c r="F17" s="14" t="n"/>
+      <c r="G17" s="14" t="n"/>
+      <c r="H17" s="14" t="n"/>
+      <c r="I17" s="15" t="n"/>
+      <c r="J17" s="25" t="n"/>
+      <c r="K17" s="17" t="n"/>
+      <c r="L17" s="26" t="n"/>
+      <c r="M17" s="26" t="n"/>
+      <c r="N17" s="26" t="n"/>
+      <c r="O17" s="26" t="n"/>
+      <c r="P17" s="26" t="n"/>
+      <c r="Q17" s="19" t="n"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="5">
         <f>A17+1</f>
         <v/>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="8" t="n">
-        <v>138</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="K18" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="24" t="n">
-        <v>0.855072463768116</v>
-      </c>
-      <c r="M18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="B18" s="6" t="n"/>
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="6" t="n"/>
+      <c r="E18" s="6" t="n"/>
+      <c r="F18" s="9" t="n"/>
+      <c r="G18" s="9" t="n"/>
+      <c r="H18" s="9" t="n"/>
+      <c r="I18" s="8" t="n"/>
+      <c r="J18" s="9" t="n"/>
+      <c r="K18" s="10" t="n"/>
+      <c r="L18" s="24" t="n"/>
+      <c r="M18" s="24" t="n"/>
+      <c r="N18" s="24" t="n"/>
+      <c r="O18" s="24" t="n"/>
+      <c r="P18" s="24" t="n"/>
+      <c r="Q18" s="12" t="n"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="5">
         <f>A18+1</f>
         <v/>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="15" t="n">
-        <v>72</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="M19" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O19" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P19" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="B19" s="13" t="n"/>
+      <c r="C19" s="13" t="n"/>
+      <c r="D19" s="13" t="n"/>
+      <c r="E19" s="13" t="n"/>
+      <c r="F19" s="14" t="n"/>
+      <c r="G19" s="14" t="n"/>
+      <c r="H19" s="14" t="n"/>
+      <c r="I19" s="15" t="n"/>
+      <c r="J19" s="25" t="n"/>
+      <c r="K19" s="17" t="n"/>
+      <c r="L19" s="26" t="n"/>
+      <c r="M19" s="26" t="n"/>
+      <c r="N19" s="26" t="n"/>
+      <c r="O19" s="26" t="n"/>
+      <c r="P19" s="26" t="n"/>
+      <c r="Q19" s="19" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="20" spans="1:17">
       <c r="A20" s="5">
         <f>A19+1</f>
         <v/>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="8" t="n">
-        <v>190</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" s="24" t="n">
-        <v>0.7631578947368421</v>
-      </c>
-      <c r="M20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P20" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="6" t="n"/>
+      <c r="D20" s="6" t="n"/>
+      <c r="E20" s="6" t="n"/>
+      <c r="F20" s="9" t="n"/>
+      <c r="G20" s="9" t="n"/>
+      <c r="H20" s="9" t="n"/>
+      <c r="I20" s="8" t="n"/>
+      <c r="J20" s="9" t="n"/>
+      <c r="K20" s="10" t="n"/>
+      <c r="L20" s="24" t="n"/>
+      <c r="M20" s="24" t="n"/>
+      <c r="N20" s="24" t="n"/>
+      <c r="O20" s="24" t="n"/>
+      <c r="P20" s="24" t="n"/>
+      <c r="Q20" s="12" t="n"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="5">
         <f>A20+1</f>
         <v/>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="15" t="n">
-        <v>149</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L21" s="26" t="n">
-        <v>0.7785234899328859</v>
-      </c>
-      <c r="M21" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O21" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P21" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q21" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="B21" s="13" t="n"/>
+      <c r="C21" s="13" t="n"/>
+      <c r="D21" s="13" t="n"/>
+      <c r="E21" s="13" t="n"/>
+      <c r="F21" s="14" t="n"/>
+      <c r="G21" s="14" t="n"/>
+      <c r="H21" s="14" t="n"/>
+      <c r="I21" s="15" t="n"/>
+      <c r="J21" s="25" t="n"/>
+      <c r="K21" s="17" t="n"/>
+      <c r="L21" s="26" t="n"/>
+      <c r="M21" s="26" t="n"/>
+      <c r="N21" s="26" t="n"/>
+      <c r="O21" s="26" t="n"/>
+      <c r="P21" s="26" t="n"/>
+      <c r="Q21" s="19" t="n"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="5">
         <f>A21+1</f>
         <v/>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="8" t="n">
-        <v>100</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="K22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" s="24" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="M22" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O22" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P22" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q22" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="6" t="n"/>
+      <c r="E22" s="6" t="n"/>
+      <c r="F22" s="9" t="n"/>
+      <c r="G22" s="9" t="n"/>
+      <c r="H22" s="9" t="n"/>
+      <c r="I22" s="8" t="n"/>
+      <c r="J22" s="9" t="n"/>
+      <c r="K22" s="10" t="n"/>
+      <c r="L22" s="24" t="n"/>
+      <c r="M22" s="24" t="n"/>
+      <c r="N22" s="24" t="n"/>
+      <c r="O22" s="24" t="n"/>
+      <c r="P22" s="24" t="n"/>
+      <c r="Q22" s="12" t="n"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="5">

</xml_diff>